<commit_message>
fazendo alterações nas mensagens
</commit_message>
<xml_diff>
--- a/planilhas/andrey_testenumeros.xlsx
+++ b/planilhas/andrey_testenumeros.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,6 +444,28 @@
           <t>codigo</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>nome</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>48998418335</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">andy </t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -453,7 +475,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>sla</t>
         </is>
       </c>
     </row>

</xml_diff>